<commit_message>
refactor|GetNewPrice|upload new price list
</commit_message>
<xml_diff>
--- a/prices_for_processing/price_sota/price_sota(xlsx)/Sota_price_bn.xlsx
+++ b/prices_for_processing/price_sota/price_sota(xlsx)/Sota_price_bn.xlsx
@@ -412,7 +412,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354" uniqueCount="914">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1353" uniqueCount="914">
   <si>
     <t>KVR16LS11S6/2</t>
   </si>
@@ -14815,7 +14815,7 @@
     <tabColor rgb="FFFFC000"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:K222"/>
+  <dimension ref="B1:V222"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="10" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
@@ -14848,7 +14848,7 @@
         <v>2</v>
       </c>
       <c r="K1" s="155">
-        <v>44623</v>
+        <v>44624</v>
       </c>
     </row>
     <row r="2" spans="2:11">
@@ -18279,18 +18279,10 @@
       </c>
       <c r="E136" s="104"/>
       <c r="F136" s="77"/>
-      <c r="G136" s="78">
-        <v>260.26</v>
-      </c>
-      <c r="H136" s="81">
-        <v>255.26</v>
-      </c>
-      <c r="I136" s="78">
-        <v>250.25</v>
-      </c>
-      <c r="J136" s="73" t="s">
-        <v>3</v>
-      </c>
+      <c r="G136" s="78"/>
+      <c r="H136" s="81"/>
+      <c r="I136" s="78"/>
+      <c r="J136" s="73"/>
       <c r="K136" s="162" t="s">
         <v>20</v>
       </c>
@@ -18512,13 +18504,13 @@
       <c r="E146" s="104"/>
       <c r="F146" s="77"/>
       <c r="G146" s="78">
-        <v>498.68</v>
+        <v>473.2</v>
       </c>
       <c r="H146" s="81">
-        <v>489.09</v>
+        <v>464.1</v>
       </c>
       <c r="I146" s="78">
-        <v>479.5</v>
+        <v>455</v>
       </c>
       <c r="J146" s="73" t="s">
         <v>3</v>
@@ -18540,13 +18532,13 @@
       <c r="E147" s="104"/>
       <c r="F147" s="77"/>
       <c r="G147" s="78">
-        <v>997.36</v>
+        <v>946.4</v>
       </c>
       <c r="H147" s="81">
-        <v>978.18</v>
+        <v>928.2</v>
       </c>
       <c r="I147" s="78">
-        <v>959</v>
+        <v>910</v>
       </c>
       <c r="J147" s="73" t="s">
         <v>3</v>
@@ -18568,13 +18560,13 @@
       <c r="E148" s="104"/>
       <c r="F148" s="77"/>
       <c r="G148" s="78">
-        <v>520.52</v>
+        <v>491.4</v>
       </c>
       <c r="H148" s="81">
-        <v>510.51</v>
+        <v>481.95</v>
       </c>
       <c r="I148" s="78">
-        <v>500.5</v>
+        <v>472.5</v>
       </c>
       <c r="J148" s="73" t="s">
         <v>3</v>
@@ -18596,13 +18588,13 @@
       <c r="E149" s="104"/>
       <c r="F149" s="77"/>
       <c r="G149" s="78">
-        <v>1041.04</v>
+        <v>982.8</v>
       </c>
       <c r="H149" s="81">
-        <v>1021.02</v>
+        <v>963.9</v>
       </c>
       <c r="I149" s="78">
-        <v>1001</v>
+        <v>945</v>
       </c>
       <c r="J149" s="73" t="s">
         <v>3</v>
@@ -18624,13 +18616,13 @@
       <c r="E150" s="104"/>
       <c r="F150" s="77"/>
       <c r="G150" s="78">
-        <v>560.55999999999995</v>
+        <v>531.44000000000005</v>
       </c>
       <c r="H150" s="81">
-        <v>549.78</v>
+        <v>521.22</v>
       </c>
       <c r="I150" s="78">
-        <v>539</v>
+        <v>511</v>
       </c>
       <c r="J150" s="73" t="s">
         <v>3</v>
@@ -18652,13 +18644,13 @@
       <c r="E151" s="104"/>
       <c r="F151" s="77"/>
       <c r="G151" s="78">
-        <v>1121.1199999999999</v>
+        <v>1062.8800000000001</v>
       </c>
       <c r="H151" s="81">
-        <v>1099.56</v>
+        <v>1042.44</v>
       </c>
       <c r="I151" s="78">
-        <v>1078</v>
+        <v>1022</v>
       </c>
       <c r="J151" s="73" t="s">
         <v>3</v>
@@ -18680,13 +18672,13 @@
       <c r="E152" s="104"/>
       <c r="F152" s="77"/>
       <c r="G152" s="78">
-        <v>637</v>
+        <v>604.24</v>
       </c>
       <c r="H152" s="81">
-        <v>624.75</v>
+        <v>592.62</v>
       </c>
       <c r="I152" s="78">
-        <v>612.5</v>
+        <v>581</v>
       </c>
       <c r="J152" s="73" t="s">
         <v>3</v>
@@ -18708,13 +18700,13 @@
       <c r="E153" s="104"/>
       <c r="F153" s="77"/>
       <c r="G153" s="78">
-        <v>1274</v>
+        <v>1208.48</v>
       </c>
       <c r="H153" s="81">
-        <v>1249.5</v>
+        <v>1185.24</v>
       </c>
       <c r="I153" s="78">
-        <v>1225</v>
+        <v>1162</v>
       </c>
       <c r="J153" s="73" t="s">
         <v>3</v>

</xml_diff>